<commit_message>
new data, new figs
</commit_message>
<xml_diff>
--- a/case_study_analysis/cf_scripts/data/raw/Mar 19_Copy of Yuga and Gaku@Japan SNAPP Case Study  - March 19, 10_03 AM.xlsx
+++ b/case_study_analysis/cf_scripts/data/raw/Mar 19_Copy of Yuga and Gaku@Japan SNAPP Case Study  - March 19, 10_03 AM.xlsx
@@ -7131,7 +7131,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image4.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7187,7 +7187,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7215,7 +7215,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>